<commit_message>
started working on conditions for strohmstead
</commit_message>
<xml_diff>
--- a/documentation/cards-2e.xlsx
+++ b/documentation/cards-2e.xlsx
@@ -132,9 +132,6 @@
     <t>Rivers and Streams</t>
   </si>
   <si>
-    <t>Strohmstead</t>
-  </si>
-  <si>
     <t>American Ginseng</t>
   </si>
   <si>
@@ -1018,6 +1015,9 @@
   </si>
   <si>
     <t>0011_2014-FOREST-06.jpg</t>
+  </si>
+  <si>
+    <t>The Strohmstead</t>
   </si>
 </sst>
 </file>
@@ -1337,9 +1337,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V7" sqref="V7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1431,10 +1431,10 @@
         <v>33</v>
       </c>
       <c r="V1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -1445,7 +1445,7 @@
         <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1454,7 +1454,7 @@
         <v>26</v>
       </c>
       <c r="V2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -1465,7 +1465,7 @@
         <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1474,7 +1474,7 @@
         <v>26</v>
       </c>
       <c r="V3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
@@ -1485,7 +1485,7 @@
         <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1494,7 +1494,7 @@
         <v>26</v>
       </c>
       <c r="V4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
@@ -1505,7 +1505,7 @@
         <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1514,7 +1514,7 @@
         <v>26</v>
       </c>
       <c r="V5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -1525,7 +1525,7 @@
         <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1534,7 +1534,7 @@
         <v>26</v>
       </c>
       <c r="V6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -1545,7 +1545,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1554,7 +1554,7 @@
         <v>26</v>
       </c>
       <c r="V7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -1565,7 +1565,7 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1574,7 +1574,7 @@
         <v>26</v>
       </c>
       <c r="V8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
@@ -1585,7 +1585,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1594,7 +1594,7 @@
         <v>26</v>
       </c>
       <c r="V9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
@@ -1605,7 +1605,7 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1614,7 +1614,7 @@
         <v>26</v>
       </c>
       <c r="V10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
@@ -1625,7 +1625,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1634,7 +1634,7 @@
         <v>26</v>
       </c>
       <c r="V11" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
@@ -1645,7 +1645,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1654,7 +1654,7 @@
         <v>26</v>
       </c>
       <c r="V12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
@@ -1665,7 +1665,7 @@
         <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1674,7 +1674,7 @@
         <v>26</v>
       </c>
       <c r="V13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -1685,7 +1685,7 @@
         <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1694,7 +1694,7 @@
         <v>26</v>
       </c>
       <c r="V14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
@@ -1705,7 +1705,7 @@
         <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1714,7 +1714,7 @@
         <v>26</v>
       </c>
       <c r="V15" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
@@ -1725,7 +1725,7 @@
         <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1734,7 +1734,7 @@
         <v>26</v>
       </c>
       <c r="V16" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
@@ -1745,7 +1745,7 @@
         <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1754,7 +1754,7 @@
         <v>26</v>
       </c>
       <c r="V17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
@@ -1765,7 +1765,7 @@
         <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1774,7 +1774,7 @@
         <v>26</v>
       </c>
       <c r="V18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
@@ -1785,7 +1785,7 @@
         <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1794,7 +1794,7 @@
         <v>26</v>
       </c>
       <c r="V19" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
@@ -1805,7 +1805,7 @@
         <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1814,7 +1814,7 @@
         <v>26</v>
       </c>
       <c r="V20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
@@ -1825,7 +1825,7 @@
         <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1834,7 +1834,7 @@
         <v>26</v>
       </c>
       <c r="V21" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
@@ -1845,7 +1845,7 @@
         <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1854,7 +1854,7 @@
         <v>26</v>
       </c>
       <c r="V22" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
@@ -1862,10 +1862,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>330</v>
       </c>
       <c r="C23" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1874,7 +1874,7 @@
         <v>26</v>
       </c>
       <c r="V23" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
@@ -1882,7 +1882,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
@@ -1894,19 +1894,19 @@
         <v>26</v>
       </c>
       <c r="G24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="V24" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="W24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
@@ -1914,7 +1914,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>
@@ -1926,19 +1926,19 @@
         <v>26</v>
       </c>
       <c r="G25" t="s">
+        <v>43</v>
+      </c>
+      <c r="H25" t="s">
+        <v>37</v>
+      </c>
+      <c r="U25" t="s">
         <v>44</v>
       </c>
-      <c r="H25" t="s">
-        <v>38</v>
-      </c>
-      <c r="U25" t="s">
+      <c r="V25" t="s">
         <v>45</v>
       </c>
-      <c r="V25" t="s">
+      <c r="W25" t="s">
         <v>46</v>
-      </c>
-      <c r="W25" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
@@ -1946,7 +1946,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26" t="s">
         <v>17</v>
@@ -1958,25 +1958,25 @@
         <v>26</v>
       </c>
       <c r="G26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H26" t="s">
+        <v>48</v>
+      </c>
+      <c r="I26" t="s">
+        <v>43</v>
+      </c>
+      <c r="J26" t="s">
+        <v>37</v>
+      </c>
+      <c r="U26" t="s">
         <v>49</v>
       </c>
-      <c r="I26" t="s">
-        <v>44</v>
-      </c>
-      <c r="J26" t="s">
-        <v>38</v>
-      </c>
-      <c r="U26" t="s">
+      <c r="V26" t="s">
         <v>50</v>
       </c>
-      <c r="V26" t="s">
+      <c r="W26" t="s">
         <v>51</v>
-      </c>
-      <c r="W26" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
@@ -1984,7 +1984,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
         <v>17</v>
@@ -1996,25 +1996,25 @@
         <v>26</v>
       </c>
       <c r="G27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V27" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="W27" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
@@ -2022,7 +2022,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
         <v>17</v>
@@ -2034,25 +2034,25 @@
         <v>26</v>
       </c>
       <c r="G28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U28" t="s">
+        <v>55</v>
+      </c>
+      <c r="V28" t="s">
         <v>56</v>
       </c>
-      <c r="V28" t="s">
-        <v>57</v>
-      </c>
       <c r="W28" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
@@ -2060,7 +2060,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C29" t="s">
         <v>17</v>
@@ -2072,19 +2072,19 @@
         <v>26</v>
       </c>
       <c r="G29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U29" t="s">
+        <v>58</v>
+      </c>
+      <c r="V29" t="s">
+        <v>281</v>
+      </c>
+      <c r="W29" t="s">
         <v>59</v>
-      </c>
-      <c r="V29" t="s">
-        <v>282</v>
-      </c>
-      <c r="W29" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
@@ -2092,7 +2092,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>
@@ -2104,19 +2104,19 @@
         <v>26</v>
       </c>
       <c r="G30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U30" t="s">
+        <v>61</v>
+      </c>
+      <c r="V30" t="s">
+        <v>282</v>
+      </c>
+      <c r="W30" t="s">
         <v>62</v>
-      </c>
-      <c r="V30" t="s">
-        <v>283</v>
-      </c>
-      <c r="W30" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
@@ -2124,7 +2124,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C31" t="s">
         <v>17</v>
@@ -2136,25 +2136,25 @@
         <v>26</v>
       </c>
       <c r="G31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U31" t="s">
+        <v>64</v>
+      </c>
+      <c r="V31" t="s">
         <v>65</v>
       </c>
-      <c r="V31" t="s">
+      <c r="W31" t="s">
         <v>66</v>
-      </c>
-      <c r="W31" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
@@ -2162,7 +2162,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" t="s">
         <v>17</v>
@@ -2174,25 +2174,25 @@
         <v>26</v>
       </c>
       <c r="G32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="V32" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="W32" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
@@ -2200,7 +2200,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C33" t="s">
         <v>17</v>
@@ -2212,25 +2212,25 @@
         <v>26</v>
       </c>
       <c r="G33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U33" t="s">
+        <v>70</v>
+      </c>
+      <c r="V33" t="s">
+        <v>284</v>
+      </c>
+      <c r="W33" t="s">
         <v>71</v>
-      </c>
-      <c r="V33" t="s">
-        <v>285</v>
-      </c>
-      <c r="W33" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
@@ -2238,7 +2238,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C34" t="s">
         <v>17</v>
@@ -2250,25 +2250,25 @@
         <v>26</v>
       </c>
       <c r="G34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V34" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="W34" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
@@ -2276,7 +2276,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C35" t="s">
         <v>17</v>
@@ -2288,25 +2288,25 @@
         <v>26</v>
       </c>
       <c r="G35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U35" t="s">
+        <v>74</v>
+      </c>
+      <c r="V35" t="s">
         <v>75</v>
       </c>
-      <c r="V35" t="s">
-        <v>76</v>
-      </c>
       <c r="W35" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
@@ -2314,7 +2314,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C36" t="s">
         <v>18</v>
@@ -2326,25 +2326,25 @@
         <v>26</v>
       </c>
       <c r="G36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U36" t="s">
+        <v>77</v>
+      </c>
+      <c r="V36" t="s">
+        <v>286</v>
+      </c>
+      <c r="W36" t="s">
         <v>78</v>
-      </c>
-      <c r="V36" t="s">
-        <v>287</v>
-      </c>
-      <c r="W36" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
@@ -2352,7 +2352,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C37" t="s">
         <v>18</v>
@@ -2364,19 +2364,19 @@
         <v>26</v>
       </c>
       <c r="G37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="U37" t="s">
+        <v>81</v>
+      </c>
+      <c r="V37" t="s">
+        <v>287</v>
+      </c>
+      <c r="W37" t="s">
         <v>82</v>
-      </c>
-      <c r="V37" t="s">
-        <v>288</v>
-      </c>
-      <c r="W37" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
@@ -2384,7 +2384,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C38" t="s">
         <v>18</v>
@@ -2396,25 +2396,25 @@
         <v>26</v>
       </c>
       <c r="G38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U38" t="s">
+        <v>84</v>
+      </c>
+      <c r="V38" t="s">
+        <v>288</v>
+      </c>
+      <c r="W38" t="s">
         <v>85</v>
-      </c>
-      <c r="V38" t="s">
-        <v>289</v>
-      </c>
-      <c r="W38" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
@@ -2422,7 +2422,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C39" t="s">
         <v>18</v>
@@ -2434,25 +2434,25 @@
         <v>26</v>
       </c>
       <c r="G39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="V39" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="W39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.25">
@@ -2460,7 +2460,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C40" t="s">
         <v>18</v>
@@ -2472,25 +2472,25 @@
         <v>26</v>
       </c>
       <c r="G40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U40" t="s">
+        <v>90</v>
+      </c>
+      <c r="V40" t="s">
+        <v>290</v>
+      </c>
+      <c r="W40" t="s">
         <v>91</v>
-      </c>
-      <c r="V40" t="s">
-        <v>291</v>
-      </c>
-      <c r="W40" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.25">
@@ -2498,7 +2498,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C41" t="s">
         <v>18</v>
@@ -2510,19 +2510,19 @@
         <v>26</v>
       </c>
       <c r="G41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="U41" t="s">
+        <v>92</v>
+      </c>
+      <c r="V41" t="s">
+        <v>291</v>
+      </c>
+      <c r="W41" t="s">
         <v>93</v>
-      </c>
-      <c r="V41" t="s">
-        <v>292</v>
-      </c>
-      <c r="W41" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.25">
@@ -2530,43 +2530,43 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C42" t="s">
+        <v>94</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" t="s">
         <v>95</v>
       </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-      <c r="E42" t="s">
-        <v>96</v>
-      </c>
       <c r="G42" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K42" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L42">
         <v>4</v>
       </c>
       <c r="U42" t="s">
+        <v>97</v>
+      </c>
+      <c r="V42" t="s">
+        <v>292</v>
+      </c>
+      <c r="W42" t="s">
         <v>98</v>
-      </c>
-      <c r="V42" t="s">
-        <v>293</v>
-      </c>
-      <c r="W42" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.25">
@@ -2574,49 +2574,49 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C43" t="s">
+        <v>94</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
         <v>95</v>
       </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="E43" t="s">
-        <v>96</v>
-      </c>
       <c r="G43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H43" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K43" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L43">
         <v>4</v>
       </c>
       <c r="M43" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N43">
         <v>5</v>
       </c>
       <c r="U43" t="s">
+        <v>100</v>
+      </c>
+      <c r="V43" t="s">
+        <v>293</v>
+      </c>
+      <c r="W43" t="s">
         <v>101</v>
-      </c>
-      <c r="V43" t="s">
-        <v>294</v>
-      </c>
-      <c r="W43" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
@@ -2624,49 +2624,49 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C44" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
         <v>95</v>
       </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44" t="s">
-        <v>96</v>
-      </c>
       <c r="G44" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K44" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L44">
         <v>4</v>
       </c>
       <c r="M44" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N44">
         <v>5</v>
       </c>
       <c r="U44" t="s">
+        <v>103</v>
+      </c>
+      <c r="V44" t="s">
         <v>104</v>
       </c>
-      <c r="V44" t="s">
+      <c r="W44" t="s">
         <v>105</v>
-      </c>
-      <c r="W44" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.25">
@@ -2674,43 +2674,43 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C45" t="s">
+        <v>94</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
         <v>95</v>
       </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-      <c r="E45" t="s">
-        <v>96</v>
-      </c>
       <c r="G45" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K45" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L45">
         <v>4</v>
       </c>
       <c r="U45" t="s">
+        <v>107</v>
+      </c>
+      <c r="V45" t="s">
         <v>108</v>
       </c>
-      <c r="V45" t="s">
-        <v>109</v>
-      </c>
       <c r="W45" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.25">
@@ -2718,43 +2718,43 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C46" t="s">
+        <v>94</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
         <v>95</v>
       </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-      <c r="E46" t="s">
-        <v>96</v>
-      </c>
       <c r="G46" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L46">
         <v>5</v>
       </c>
       <c r="U46" t="s">
+        <v>110</v>
+      </c>
+      <c r="V46" t="s">
+        <v>294</v>
+      </c>
+      <c r="W46" t="s">
         <v>111</v>
-      </c>
-      <c r="V46" t="s">
-        <v>295</v>
-      </c>
-      <c r="W46" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.25">
@@ -2762,43 +2762,43 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C47" t="s">
+        <v>94</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47" t="s">
         <v>95</v>
       </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-      <c r="E47" t="s">
-        <v>96</v>
-      </c>
       <c r="G47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J47" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K47" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L47">
         <v>4</v>
       </c>
       <c r="U47" t="s">
+        <v>113</v>
+      </c>
+      <c r="V47" t="s">
         <v>114</v>
       </c>
-      <c r="V47" t="s">
+      <c r="W47" t="s">
         <v>115</v>
-      </c>
-      <c r="W47" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.25">
@@ -2806,49 +2806,49 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C48" t="s">
+        <v>94</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48" t="s">
         <v>95</v>
       </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
-      <c r="E48" t="s">
-        <v>96</v>
-      </c>
       <c r="G48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K48" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L48">
         <v>4</v>
       </c>
       <c r="M48" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N48">
         <v>5</v>
       </c>
       <c r="U48" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="V48" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="W48" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.25">
@@ -2856,43 +2856,43 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C49" t="s">
+        <v>94</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49" t="s">
         <v>95</v>
       </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="E49" t="s">
-        <v>96</v>
-      </c>
       <c r="G49" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J49" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K49" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L49">
         <v>4</v>
       </c>
       <c r="U49" t="s">
+        <v>119</v>
+      </c>
+      <c r="V49" t="s">
+        <v>296</v>
+      </c>
+      <c r="W49" t="s">
         <v>120</v>
-      </c>
-      <c r="V49" t="s">
-        <v>297</v>
-      </c>
-      <c r="W49" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.25">
@@ -2900,49 +2900,49 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C50" t="s">
+        <v>94</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50" t="s">
         <v>95</v>
       </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-      <c r="E50" t="s">
-        <v>96</v>
-      </c>
       <c r="G50" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I50" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J50" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K50" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L50">
         <v>4</v>
       </c>
       <c r="M50" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N50">
         <v>5</v>
       </c>
       <c r="U50" t="s">
+        <v>122</v>
+      </c>
+      <c r="V50" t="s">
         <v>123</v>
       </c>
-      <c r="V50" t="s">
+      <c r="W50" t="s">
         <v>124</v>
-      </c>
-      <c r="W50" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.25">
@@ -2950,49 +2950,49 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C51" t="s">
+        <v>94</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51" t="s">
         <v>95</v>
       </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
-      <c r="E51" t="s">
-        <v>96</v>
-      </c>
       <c r="G51" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I51" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J51" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K51" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L51">
         <v>4</v>
       </c>
       <c r="M51" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N51">
         <v>5</v>
       </c>
       <c r="U51" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="V51" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="W51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.25">
@@ -3000,43 +3000,43 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C52" t="s">
+        <v>94</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52" t="s">
         <v>95</v>
       </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-      <c r="E52" t="s">
-        <v>96</v>
-      </c>
       <c r="G52" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I52" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J52" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K52" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L52">
         <v>4</v>
       </c>
       <c r="U52" t="s">
+        <v>128</v>
+      </c>
+      <c r="V52" t="s">
+        <v>298</v>
+      </c>
+      <c r="W52" t="s">
         <v>129</v>
-      </c>
-      <c r="V52" t="s">
-        <v>299</v>
-      </c>
-      <c r="W52" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.25">
@@ -3044,43 +3044,43 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C53" t="s">
+        <v>94</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53" t="s">
         <v>95</v>
       </c>
-      <c r="D53">
-        <v>1</v>
-      </c>
-      <c r="E53" t="s">
-        <v>96</v>
-      </c>
       <c r="G53" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I53" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J53" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K53" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L53">
         <v>4</v>
       </c>
       <c r="U53" t="s">
+        <v>131</v>
+      </c>
+      <c r="V53" t="s">
+        <v>299</v>
+      </c>
+      <c r="W53" t="s">
         <v>132</v>
-      </c>
-      <c r="V53" t="s">
-        <v>300</v>
-      </c>
-      <c r="W53" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.25">
@@ -3088,37 +3088,37 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C54" t="s">
+        <v>94</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54" t="s">
         <v>95</v>
       </c>
-      <c r="D54">
-        <v>1</v>
-      </c>
-      <c r="E54" t="s">
-        <v>96</v>
-      </c>
       <c r="G54" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H54" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K54" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L54">
         <v>4</v>
       </c>
       <c r="U54" t="s">
+        <v>133</v>
+      </c>
+      <c r="V54" t="s">
+        <v>300</v>
+      </c>
+      <c r="W54" t="s">
         <v>134</v>
-      </c>
-      <c r="V54" t="s">
-        <v>301</v>
-      </c>
-      <c r="W54" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.25">
@@ -3126,49 +3126,49 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C55" t="s">
+        <v>94</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55" t="s">
         <v>95</v>
       </c>
-      <c r="D55">
-        <v>1</v>
-      </c>
-      <c r="E55" t="s">
-        <v>96</v>
-      </c>
       <c r="G55" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H55" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I55" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J55" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K55" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L55">
         <v>4</v>
       </c>
       <c r="M55" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N55">
         <v>5</v>
       </c>
       <c r="U55" t="s">
+        <v>137</v>
+      </c>
+      <c r="V55" t="s">
+        <v>301</v>
+      </c>
+      <c r="W55" t="s">
         <v>138</v>
-      </c>
-      <c r="V55" t="s">
-        <v>302</v>
-      </c>
-      <c r="W55" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.25">
@@ -3176,34 +3176,34 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C56" t="s">
+        <v>94</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56" t="s">
         <v>95</v>
       </c>
-      <c r="D56">
-        <v>1</v>
-      </c>
-      <c r="E56" t="s">
-        <v>96</v>
-      </c>
       <c r="G56" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K56" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L56">
         <v>4</v>
       </c>
       <c r="U56" t="s">
+        <v>140</v>
+      </c>
+      <c r="V56" t="s">
+        <v>302</v>
+      </c>
+      <c r="W56" t="s">
         <v>141</v>
-      </c>
-      <c r="V56" t="s">
-        <v>303</v>
-      </c>
-      <c r="W56" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.25">
@@ -3211,37 +3211,37 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C57" t="s">
+        <v>94</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57" t="s">
         <v>95</v>
       </c>
-      <c r="D57">
-        <v>1</v>
-      </c>
-      <c r="E57" t="s">
-        <v>96</v>
-      </c>
       <c r="G57" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H57" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K57" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L57">
         <v>5</v>
       </c>
       <c r="U57" t="s">
+        <v>143</v>
+      </c>
+      <c r="V57" t="s">
+        <v>303</v>
+      </c>
+      <c r="W57" t="s">
         <v>144</v>
-      </c>
-      <c r="V57" t="s">
-        <v>304</v>
-      </c>
-      <c r="W57" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.25">
@@ -3249,37 +3249,37 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C58" t="s">
+        <v>94</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58" t="s">
         <v>95</v>
       </c>
-      <c r="D58">
-        <v>1</v>
-      </c>
-      <c r="E58" t="s">
-        <v>96</v>
-      </c>
       <c r="G58" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H58" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K58" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L58">
         <v>5</v>
       </c>
       <c r="U58" t="s">
+        <v>146</v>
+      </c>
+      <c r="V58" t="s">
+        <v>304</v>
+      </c>
+      <c r="W58" t="s">
         <v>147</v>
-      </c>
-      <c r="V58" t="s">
-        <v>305</v>
-      </c>
-      <c r="W58" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.25">
@@ -3287,49 +3287,49 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D59">
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G59" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H59" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I59" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J59" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K59" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L59">
         <v>7</v>
       </c>
       <c r="M59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N59">
         <v>8</v>
       </c>
       <c r="U59" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="V59" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="W59" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.25">
@@ -3337,37 +3337,37 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C60" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D60">
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G60" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H60" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K60" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="L60">
         <v>8</v>
       </c>
       <c r="U60" t="s">
+        <v>151</v>
+      </c>
+      <c r="V60" t="s">
+        <v>306</v>
+      </c>
+      <c r="W60" t="s">
         <v>152</v>
-      </c>
-      <c r="V60" t="s">
-        <v>307</v>
-      </c>
-      <c r="W60" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.25">
@@ -3375,49 +3375,49 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C61" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D61">
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G61" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H61" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K61" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L61">
         <v>6</v>
       </c>
       <c r="M61" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N61">
         <v>7</v>
       </c>
       <c r="O61" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="P61">
         <v>8</v>
       </c>
       <c r="U61" t="s">
+        <v>154</v>
+      </c>
+      <c r="V61" t="s">
         <v>155</v>
       </c>
-      <c r="V61" t="s">
+      <c r="W61" t="s">
         <v>156</v>
-      </c>
-      <c r="W61" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.25">
@@ -3425,43 +3425,43 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C62" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D62">
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H62" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K62" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L62">
         <v>7</v>
       </c>
       <c r="M62" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N62">
         <v>8</v>
       </c>
       <c r="U62" t="s">
+        <v>158</v>
+      </c>
+      <c r="V62" t="s">
         <v>159</v>
       </c>
-      <c r="V62" t="s">
+      <c r="W62" t="s">
         <v>160</v>
-      </c>
-      <c r="W62" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.25">
@@ -3469,49 +3469,49 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C63" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D63">
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G63" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H63" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I63" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J63" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K63" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L63">
         <v>7</v>
       </c>
       <c r="M63" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N63">
         <v>8</v>
       </c>
       <c r="U63" t="s">
+        <v>162</v>
+      </c>
+      <c r="V63" t="s">
         <v>163</v>
       </c>
-      <c r="V63" t="s">
+      <c r="W63" t="s">
         <v>164</v>
-      </c>
-      <c r="W63" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.25">
@@ -3519,61 +3519,61 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C64" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D64">
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G64" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H64" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I64" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J64" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K64" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L64">
         <v>6</v>
       </c>
       <c r="M64" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N64">
         <v>7</v>
       </c>
       <c r="O64" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="P64">
         <v>8</v>
       </c>
       <c r="Q64" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="R64">
         <v>9</v>
       </c>
       <c r="U64" t="s">
+        <v>166</v>
+      </c>
+      <c r="V64" t="s">
+        <v>307</v>
+      </c>
+      <c r="W64" t="s">
         <v>167</v>
-      </c>
-      <c r="V64" t="s">
-        <v>308</v>
-      </c>
-      <c r="W64" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="65" spans="1:23" x14ac:dyDescent="0.25">
@@ -3581,43 +3581,43 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C65" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D65">
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G65" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I65" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J65" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K65" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L65">
         <v>7</v>
       </c>
       <c r="U65" t="s">
+        <v>169</v>
+      </c>
+      <c r="V65" t="s">
+        <v>308</v>
+      </c>
+      <c r="W65" t="s">
         <v>170</v>
-      </c>
-      <c r="V65" t="s">
-        <v>309</v>
-      </c>
-      <c r="W65" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="66" spans="1:23" x14ac:dyDescent="0.25">
@@ -3625,49 +3625,49 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C66" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D66">
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G66" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H66" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I66" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J66" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K66" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L66">
         <v>7</v>
       </c>
       <c r="M66" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N66">
         <v>8</v>
       </c>
       <c r="U66" t="s">
+        <v>172</v>
+      </c>
+      <c r="V66" t="s">
+        <v>309</v>
+      </c>
+      <c r="W66" t="s">
         <v>173</v>
-      </c>
-      <c r="V66" t="s">
-        <v>310</v>
-      </c>
-      <c r="W66" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="67" spans="1:23" x14ac:dyDescent="0.25">
@@ -3675,43 +3675,43 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C67" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D67">
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G67" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H67" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K67" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L67">
         <v>6</v>
       </c>
       <c r="M67" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N67">
         <v>7</v>
       </c>
       <c r="U67" t="s">
+        <v>175</v>
+      </c>
+      <c r="V67" t="s">
         <v>176</v>
       </c>
-      <c r="V67" t="s">
+      <c r="W67" t="s">
         <v>177</v>
-      </c>
-      <c r="W67" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="68" spans="1:23" x14ac:dyDescent="0.25">
@@ -3719,49 +3719,49 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C68" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D68">
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G68" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H68" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K68" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L68">
         <v>6</v>
       </c>
       <c r="M68" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N68">
         <v>7</v>
       </c>
       <c r="O68" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="P68">
         <v>8</v>
       </c>
       <c r="U68" t="s">
+        <v>179</v>
+      </c>
+      <c r="V68" t="s">
+        <v>310</v>
+      </c>
+      <c r="W68" t="s">
         <v>180</v>
-      </c>
-      <c r="V68" t="s">
-        <v>311</v>
-      </c>
-      <c r="W68" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="69" spans="1:23" x14ac:dyDescent="0.25">
@@ -3769,34 +3769,34 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C69" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D69">
         <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G69" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K69" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L69">
         <v>6</v>
       </c>
       <c r="U69" t="s">
+        <v>182</v>
+      </c>
+      <c r="V69" t="s">
+        <v>311</v>
+      </c>
+      <c r="W69" t="s">
         <v>183</v>
-      </c>
-      <c r="V69" t="s">
-        <v>312</v>
-      </c>
-      <c r="W69" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="70" spans="1:23" x14ac:dyDescent="0.25">
@@ -3804,55 +3804,55 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C70" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D70">
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G70" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H70" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I70" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J70" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K70" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L70">
         <v>6</v>
       </c>
       <c r="M70" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N70">
         <v>7</v>
       </c>
       <c r="O70" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="P70">
         <v>8</v>
       </c>
       <c r="U70" t="s">
+        <v>185</v>
+      </c>
+      <c r="V70" t="s">
         <v>186</v>
       </c>
-      <c r="V70" t="s">
+      <c r="W70" t="s">
         <v>187</v>
-      </c>
-      <c r="W70" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="71" spans="1:23" x14ac:dyDescent="0.25">
@@ -3860,49 +3860,49 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C71" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D71">
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G71" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H71" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I71" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J71" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K71" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L71">
         <v>6</v>
       </c>
       <c r="M71" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N71">
         <v>7</v>
       </c>
       <c r="U71" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="V71" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="W71" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="72" spans="1:23" x14ac:dyDescent="0.25">
@@ -3910,55 +3910,55 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C72" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D72">
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G72" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H72" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I72" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J72" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K72" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L72">
         <v>6</v>
       </c>
       <c r="M72" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N72">
         <v>7</v>
       </c>
       <c r="O72" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="P72">
         <v>8</v>
       </c>
       <c r="U72" t="s">
+        <v>191</v>
+      </c>
+      <c r="V72" t="s">
+        <v>313</v>
+      </c>
+      <c r="W72" t="s">
         <v>192</v>
-      </c>
-      <c r="V72" t="s">
-        <v>314</v>
-      </c>
-      <c r="W72" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="73" spans="1:23" x14ac:dyDescent="0.25">
@@ -3966,61 +3966,61 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C73" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D73">
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G73" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H73" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I73" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J73" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K73" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L73">
         <v>6</v>
       </c>
       <c r="M73" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N73">
         <v>7</v>
       </c>
       <c r="O73" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="P73">
         <v>8</v>
       </c>
       <c r="Q73" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="R73">
         <v>9</v>
       </c>
       <c r="U73" t="s">
+        <v>194</v>
+      </c>
+      <c r="V73" t="s">
+        <v>314</v>
+      </c>
+      <c r="W73" t="s">
         <v>195</v>
-      </c>
-      <c r="V73" t="s">
-        <v>315</v>
-      </c>
-      <c r="W73" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="74" spans="1:23" x14ac:dyDescent="0.25">
@@ -4028,49 +4028,49 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C74" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D74">
         <v>1</v>
       </c>
       <c r="E74" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G74" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H74" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K74" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L74">
         <v>7</v>
       </c>
       <c r="M74" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N74">
         <v>8</v>
       </c>
       <c r="O74" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="P74">
         <v>9</v>
       </c>
       <c r="U74" t="s">
+        <v>197</v>
+      </c>
+      <c r="V74" t="s">
+        <v>202</v>
+      </c>
+      <c r="W74" t="s">
         <v>198</v>
-      </c>
-      <c r="V74" t="s">
-        <v>203</v>
-      </c>
-      <c r="W74" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="75" spans="1:23" x14ac:dyDescent="0.25">
@@ -4078,61 +4078,61 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C75" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D75">
         <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G75" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H75" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I75" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J75" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K75" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L75">
         <v>6</v>
       </c>
       <c r="M75" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N75">
         <v>7</v>
       </c>
       <c r="O75" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="P75">
         <v>8</v>
       </c>
       <c r="Q75" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="R75">
         <v>9</v>
       </c>
       <c r="U75" t="s">
+        <v>200</v>
+      </c>
+      <c r="V75" t="s">
         <v>201</v>
       </c>
-      <c r="V75" t="s">
-        <v>202</v>
-      </c>
       <c r="W75" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="76" spans="1:23" x14ac:dyDescent="0.25">
@@ -4140,34 +4140,34 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C76" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D76">
         <v>1</v>
       </c>
       <c r="E76" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G76" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K76" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L76">
         <v>6</v>
       </c>
       <c r="U76" t="s">
+        <v>205</v>
+      </c>
+      <c r="V76" t="s">
         <v>206</v>
       </c>
-      <c r="V76" t="s">
+      <c r="W76" t="s">
         <v>207</v>
-      </c>
-      <c r="W76" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="77" spans="1:23" x14ac:dyDescent="0.25">
@@ -4175,46 +4175,46 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C77" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D77">
         <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G77" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H77" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I77" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K77" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L77">
         <v>7</v>
       </c>
       <c r="M77" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N77">
         <v>8</v>
       </c>
       <c r="U77" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="V77" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="W77" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="78" spans="1:23" x14ac:dyDescent="0.25">
@@ -4222,46 +4222,46 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C78" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D78">
         <v>1</v>
       </c>
       <c r="E78" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G78" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H78" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I78" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K78" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="L78">
         <v>8</v>
       </c>
       <c r="M78" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="N78">
         <v>9</v>
       </c>
       <c r="U78" t="s">
+        <v>211</v>
+      </c>
+      <c r="V78" t="s">
+        <v>316</v>
+      </c>
+      <c r="W78" t="s">
         <v>212</v>
-      </c>
-      <c r="V78" t="s">
-        <v>317</v>
-      </c>
-      <c r="W78" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="79" spans="1:23" x14ac:dyDescent="0.25">
@@ -4269,40 +4269,40 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C79" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D79">
         <v>1</v>
       </c>
       <c r="E79" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G79" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H79" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I79" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K79" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L79">
         <v>6</v>
       </c>
       <c r="U79" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="V79" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="W79" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="80" spans="1:23" x14ac:dyDescent="0.25">
@@ -4310,49 +4310,49 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C80" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D80">
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G80" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H80" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K80" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L80">
         <v>6</v>
       </c>
       <c r="M80" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N80">
         <v>7</v>
       </c>
       <c r="O80" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="P80">
         <v>8</v>
       </c>
       <c r="U80" t="s">
+        <v>216</v>
+      </c>
+      <c r="V80" t="s">
+        <v>318</v>
+      </c>
+      <c r="W80" t="s">
         <v>217</v>
-      </c>
-      <c r="V80" t="s">
-        <v>319</v>
-      </c>
-      <c r="W80" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="81" spans="1:23" x14ac:dyDescent="0.25">
@@ -4360,43 +4360,43 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
+        <v>218</v>
+      </c>
+      <c r="C81" t="s">
         <v>219</v>
       </c>
-      <c r="C81" t="s">
-        <v>220</v>
-      </c>
       <c r="D81">
         <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G81" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H81" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K81" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L81">
         <v>7</v>
       </c>
       <c r="M81" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N81">
         <v>8</v>
       </c>
       <c r="U81" t="s">
+        <v>220</v>
+      </c>
+      <c r="V81" t="s">
         <v>221</v>
       </c>
-      <c r="V81" t="s">
+      <c r="W81" t="s">
         <v>222</v>
-      </c>
-      <c r="W81" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="82" spans="1:23" x14ac:dyDescent="0.25">
@@ -4404,49 +4404,49 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C82" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D82">
         <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G82" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H82" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I82" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J82" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K82" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="L82">
         <v>8</v>
       </c>
       <c r="M82" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="N82">
         <v>9</v>
       </c>
       <c r="U82" t="s">
+        <v>224</v>
+      </c>
+      <c r="V82" t="s">
+        <v>319</v>
+      </c>
+      <c r="W82" t="s">
         <v>225</v>
-      </c>
-      <c r="V82" t="s">
-        <v>320</v>
-      </c>
-      <c r="W82" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="83" spans="1:23" x14ac:dyDescent="0.25">
@@ -4454,61 +4454,61 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C83" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D83">
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G83" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H83" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I83" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J83" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K83" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L83">
         <v>6</v>
       </c>
       <c r="M83" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N83">
         <v>7</v>
       </c>
       <c r="O83" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="P83">
         <v>8</v>
       </c>
       <c r="Q83" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="R83">
         <v>9</v>
       </c>
       <c r="U83" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V83" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="W83" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="84" spans="1:23" x14ac:dyDescent="0.25">
@@ -4516,49 +4516,49 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C84" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D84">
         <v>1</v>
       </c>
       <c r="E84" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G84" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H84" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K84" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L84">
         <v>7</v>
       </c>
       <c r="M84" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N84">
         <v>8</v>
       </c>
       <c r="O84" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="P84">
         <v>9</v>
       </c>
       <c r="U84" t="s">
+        <v>228</v>
+      </c>
+      <c r="V84" t="s">
         <v>229</v>
       </c>
-      <c r="V84" t="s">
-        <v>230</v>
-      </c>
       <c r="W84" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="85" spans="1:23" x14ac:dyDescent="0.25">
@@ -4566,49 +4566,49 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C85" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D85">
         <v>1</v>
       </c>
       <c r="E85" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G85" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H85" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I85" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J85" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K85" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="L85">
         <v>8</v>
       </c>
       <c r="M85" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="N85">
         <v>9</v>
       </c>
       <c r="U85" t="s">
+        <v>231</v>
+      </c>
+      <c r="V85" t="s">
+        <v>321</v>
+      </c>
+      <c r="W85" t="s">
         <v>232</v>
-      </c>
-      <c r="V85" t="s">
-        <v>322</v>
-      </c>
-      <c r="W85" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="86" spans="1:23" x14ac:dyDescent="0.25">
@@ -4616,61 +4616,61 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C86" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D86">
         <v>1</v>
       </c>
       <c r="E86" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G86" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H86" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I86" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J86" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K86" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L86">
         <v>6</v>
       </c>
       <c r="M86" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N86">
         <v>7</v>
       </c>
       <c r="O86" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="P86">
         <v>8</v>
       </c>
       <c r="Q86" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="R86">
         <v>9</v>
       </c>
       <c r="U86" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="V86" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="W86" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="87" spans="1:23" x14ac:dyDescent="0.25">
@@ -4678,67 +4678,67 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
+        <v>235</v>
+      </c>
+      <c r="C87" t="s">
         <v>236</v>
       </c>
-      <c r="C87" t="s">
-        <v>237</v>
-      </c>
       <c r="D87">
         <v>1</v>
       </c>
       <c r="E87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G87" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H87" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I87" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J87" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K87" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L87">
         <v>6</v>
       </c>
       <c r="M87" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N87">
         <v>7</v>
       </c>
       <c r="O87" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="P87">
         <v>8</v>
       </c>
       <c r="Q87" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="R87">
         <v>9</v>
       </c>
       <c r="S87" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="T87">
         <v>10</v>
       </c>
       <c r="U87" t="s">
+        <v>237</v>
+      </c>
+      <c r="V87" t="s">
         <v>238</v>
       </c>
-      <c r="V87" t="s">
+      <c r="W87" t="s">
         <v>239</v>
-      </c>
-      <c r="W87" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="88" spans="1:23" x14ac:dyDescent="0.25">
@@ -4746,7 +4746,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C88" t="s">
         <v>10</v>
@@ -4755,16 +4755,16 @@
         <v>1</v>
       </c>
       <c r="E88" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="U88" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="V88" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="W88" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hi res images added. fixed a bug where 2 apexes in play would prevent win
</commit_message>
<xml_diff>
--- a/documentation/cards-2e.xlsx
+++ b/documentation/cards-2e.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\OneDrive\Programming\Lua\WildGame\documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13770" windowHeight="8790"/>
   </bookViews>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="328">
   <si>
     <t>Name</t>
   </si>
@@ -1313,7 +1318,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1323,9 +1328,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V22" sqref="V22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4711,12 +4716,6 @@
       <c r="R87">
         <v>9</v>
       </c>
-      <c r="S87" t="s">
-        <v>219</v>
-      </c>
-      <c r="T87">
-        <v>10</v>
-      </c>
       <c r="U87" t="s">
         <v>237</v>
       </c>

</xml_diff>

<commit_message>
added humans scoring to 10 again
</commit_message>
<xml_diff>
--- a/documentation/cards-2e.xlsx
+++ b/documentation/cards-2e.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="328">
   <si>
     <t>Name</t>
   </si>
@@ -1328,9 +1328,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B88" sqref="B88"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R89" sqref="R89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4716,6 +4716,12 @@
       <c r="R87">
         <v>9</v>
       </c>
+      <c r="S87" t="s">
+        <v>219</v>
+      </c>
+      <c r="T87">
+        <v>10</v>
+      </c>
       <c r="U87" t="s">
         <v>237</v>
       </c>

</xml_diff>